<commit_message>
Fixing Item Template for bulk operation item
</commit_message>
<xml_diff>
--- a/LinoVative.Web.Api/Resources/ExcelFiles/CreateItemTemplate.xlsx
+++ b/LinoVative.Web.Api/Resources/ExcelFiles/CreateItemTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\LinoValtiveSolutions\LinoVative.Web.Api\Resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A71AB8-0988-406F-B8BE-A9AE86262D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1273A3CB-2B60-4EEA-B629-A6A1CC5B2760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{DDEE30A6-2B18-41C6-85EB-1999D5C66F47}"/>
   </bookViews>
@@ -31,32 +31,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Item Name</t>
-  </si>
-  <si>
-    <t>Item Code</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>Sell Price</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -95,7 +69,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,43 +424,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56733355-42C7-4069-9CC5-8A34B990EF30}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="2" width="47" customWidth="1"/>
-    <col min="3" max="5" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" customWidth="1"/>
+    <col min="12" max="12" width="25.5703125" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>